<commit_message>
uradjen prvi paket raspored resursa
</commit_message>
<xml_diff>
--- a/Projekat_Faza1_ver1/2b ETF budget - Horizon2020 .xlsx
+++ b/Projekat_Faza1_ver1/2b ETF budget - Horizon2020 .xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naca\Desktop\usp\usp\Projekat_Faza1_ver1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E8CB24-C1C0-4699-92FF-C8D57F7D4B8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3120" windowWidth="21600" windowHeight="13080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3120" windowWidth="21600" windowHeight="13080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet" sheetId="1" r:id="rId1"/>
@@ -19,6 +13,7 @@
     <sheet name="Subcontracting - budzet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,42 +30,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="O13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Kampen, Jan-Joris van:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Contributions of third parties to be budgeted as personell costs or other direct costs. No indirect costs on these costs when NOT used on the premises of the benificiary.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="117">
   <si>
@@ -428,11 +387,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -493,21 +452,6 @@
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -747,7 +691,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -824,14 +768,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -840,7 +784,7 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -850,56 +794,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -908,17 +805,64 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1035,7 +979,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1078,7 +1022,7 @@
         <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1155,7 +1099,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1207,7 +1151,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1401,21 +1345,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14:O24"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,77 +1387,77 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66" t="s">
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="K4" s="66"/>
+      <c r="K4" s="47"/>
       <c r="L4" s="45"/>
-      <c r="M4" s="63" t="s">
+      <c r="M4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="64"/>
-      <c r="O4" s="65"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="50"/>
       <c r="P4" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="K5" s="66"/>
+      <c r="K5" s="47"/>
       <c r="L5" s="45"/>
-      <c r="M5" s="63" t="s">
+      <c r="M5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="64"/>
-      <c r="O5" s="65"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="50"/>
       <c r="P5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66" t="s">
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="K6" s="66"/>
+      <c r="K6" s="47"/>
       <c r="L6" s="45"/>
-      <c r="M6" s="63" t="s">
+      <c r="M6" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="64"/>
-      <c r="O6" s="65"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="50"/>
       <c r="P6" s="5">
         <v>0.7</v>
       </c>
@@ -1523,23 +1467,23 @@
       <c r="R6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="66" t="s">
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="K7" s="66"/>
+      <c r="K7" s="47"/>
       <c r="L7" s="45"/>
-      <c r="M7" s="63" t="s">
+      <c r="M7" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="64"/>
-      <c r="O7" s="65"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="50"/>
       <c r="P7" s="4">
         <v>1</v>
       </c>
@@ -1549,56 +1493,56 @@
       <c r="O8" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="68"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="68"/>
-      <c r="O10" s="68"/>
-      <c r="P10" s="68"/>
-      <c r="Q10" s="68"/>
-      <c r="R10" s="68"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52"/>
+      <c r="R10" s="52"/>
       <c r="S10" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="61" t="s">
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="61"/>
-      <c r="L12" s="61"/>
-      <c r="M12" s="61"/>
-      <c r="N12" s="61"/>
-      <c r="O12" s="61"/>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="61"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="54"/>
       <c r="S12" s="9"/>
     </row>
     <row r="13" spans="1:19" s="15" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
       <c r="D13" s="10" t="s">
         <v>14</v>
       </c>
@@ -1649,11 +1593,11 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="17">
         <v>2</v>
       </c>
@@ -1698,11 +1642,11 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
       <c r="D15" s="17">
         <v>2</v>
       </c>
@@ -1746,11 +1690,11 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
       <c r="D16" s="17">
         <v>2</v>
       </c>
@@ -1798,11 +1742,11 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="50"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -1836,11 +1780,11 @@
       <c r="S17" s="20"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17">
@@ -1884,11 +1828,11 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="50"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="59"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -1928,11 +1872,11 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="50"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
       <c r="D20" s="17">
         <v>2</v>
       </c>
@@ -1980,11 +1924,11 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="50"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17">
         <v>1</v>
@@ -2030,11 +1974,11 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="50"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17">
@@ -2078,11 +2022,11 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="50"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="59"/>
       <c r="D23" s="17">
         <v>3</v>
       </c>
@@ -2126,11 +2070,11 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="50"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
       <c r="D24" s="17">
         <v>4</v>
       </c>
@@ -2176,11 +2120,11 @@
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="17">
         <f>SUM(D14:D24)</f>
         <v>15</v>
@@ -2301,24 +2245,24 @@
       <c r="S28" s="30"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="63"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
@@ -2359,99 +2303,99 @@
       <c r="P31" s="31"/>
     </row>
     <row r="32" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="52" t="str">
+      <c r="A32" s="66" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v>participant ETF</v>
       </c>
-      <c r="B32" s="52"/>
+      <c r="B32" s="66"/>
       <c r="C32" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="55" t="s">
+      <c r="D32" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="55"/>
-      <c r="M32" s="55"/>
-      <c r="N32" s="55"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+      <c r="P32" s="56"/>
     </row>
     <row r="33" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="46"/>
+      <c r="B33" s="60"/>
       <c r="C33" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="D33" s="56" t="s">
+      <c r="D33" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="56"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
-      <c r="O33" s="56"/>
-      <c r="P33" s="56"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="69"/>
+      <c r="N33" s="69"/>
+      <c r="O33" s="69"/>
+      <c r="P33" s="69"/>
       <c r="S33" s="30"/>
     </row>
     <row r="34" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="46"/>
+      <c r="B34" s="60"/>
       <c r="C34" s="44">
         <v>92905</v>
       </c>
-      <c r="D34" s="57" t="s">
+      <c r="D34" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="57"/>
-      <c r="M34" s="57"/>
-      <c r="N34" s="57"/>
-      <c r="O34" s="57"/>
-      <c r="P34" s="57"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="61"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="61"/>
+      <c r="P34" s="61"/>
       <c r="S34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="46"/>
+      <c r="B35" s="60"/>
       <c r="C35" s="32"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="51"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="51"/>
-      <c r="O35" s="51"/>
-      <c r="P35" s="51"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="65"/>
+      <c r="K35" s="65"/>
+      <c r="L35" s="65"/>
+      <c r="M35" s="65"/>
+      <c r="N35" s="65"/>
+      <c r="O35" s="65"/>
+      <c r="P35" s="65"/>
       <c r="S35" s="30"/>
     </row>
     <row r="36" spans="1:19" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -2485,133 +2429,103 @@
       <c r="P37" s="35"/>
     </row>
     <row r="38" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="52" t="str">
+      <c r="A38" s="66" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B38" s="52"/>
+      <c r="B38" s="66"/>
       <c r="C38" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="53" t="s">
+      <c r="D38" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
-      <c r="N38" s="53"/>
-      <c r="O38" s="53"/>
-      <c r="P38" s="53"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="67"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="67"/>
+      <c r="L38" s="67"/>
+      <c r="M38" s="67"/>
+      <c r="N38" s="67"/>
+      <c r="O38" s="67"/>
+      <c r="P38" s="67"/>
     </row>
     <row r="39" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="46"/>
+      <c r="B39" s="60"/>
       <c r="C39" s="44">
         <v>16000</v>
       </c>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="E39" s="54"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="54"/>
-      <c r="M39" s="54"/>
-      <c r="N39" s="54"/>
-      <c r="O39" s="54"/>
-      <c r="P39" s="54"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="68"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="68"/>
+      <c r="J39" s="68"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="68"/>
+      <c r="M39" s="68"/>
+      <c r="N39" s="68"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="68"/>
       <c r="S39" s="30"/>
     </row>
     <row r="40" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="46"/>
+      <c r="B40" s="60"/>
       <c r="C40" s="32"/>
-      <c r="D40" s="47" t="s">
+      <c r="D40" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="47"/>
-      <c r="M40" s="47"/>
-      <c r="N40" s="47"/>
-      <c r="O40" s="47"/>
-      <c r="P40" s="47"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="64"/>
+      <c r="H40" s="64"/>
+      <c r="I40" s="64"/>
+      <c r="J40" s="64"/>
+      <c r="K40" s="64"/>
+      <c r="L40" s="64"/>
+      <c r="M40" s="64"/>
+      <c r="N40" s="64"/>
+      <c r="O40" s="64"/>
+      <c r="P40" s="64"/>
       <c r="S40" s="30"/>
     </row>
     <row r="41" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="46"/>
+      <c r="B41" s="60"/>
       <c r="C41" s="32"/>
-      <c r="D41" s="47" t="s">
+      <c r="D41" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="47"/>
-      <c r="M41" s="47"/>
-      <c r="N41" s="47"/>
-      <c r="O41" s="47"/>
-      <c r="P41" s="47"/>
+      <c r="E41" s="64"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="64"/>
+      <c r="H41" s="64"/>
+      <c r="I41" s="64"/>
+      <c r="J41" s="64"/>
+      <c r="K41" s="64"/>
+      <c r="L41" s="64"/>
+      <c r="M41" s="64"/>
+      <c r="N41" s="64"/>
+      <c r="O41" s="64"/>
+      <c r="P41" s="64"/>
       <c r="S41" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="A10:R10"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="J12:R12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:P34"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A29:P29"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="D40:P40"/>
     <mergeCell ref="A41:B41"/>
@@ -2628,6 +2542,36 @@
     <mergeCell ref="D32:P32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="D33:P33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:P34"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A29:P29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="J12:R12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="A10:R10"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="P4">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -2635,7 +2579,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6" xr:uid="{B8B90553-3DCE-4964-9656-EBD82EEBC93C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6">
       <formula1>"70%,100%"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2643,12 +2587,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P28"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
@@ -2675,7 +2618,7 @@
         <v>18120</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="162.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="162" x14ac:dyDescent="0.25">
       <c r="B4" s="37" t="s">
         <v>44</v>
       </c>
@@ -3326,14 +3269,14 @@
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I35"/>
   <sheetViews>
     <sheetView zoomScale="65" zoomScaleNormal="95" workbookViewId="0">
@@ -3971,7 +3914,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I33"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">

</xml_diff>